<commit_message>
Adding train test data spreadsheet
</commit_message>
<xml_diff>
--- a/patient_statistics.xlsx
+++ b/patient_statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameenislam/Documents/MSc_Project/code.nosync/chbmit-seizure-prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B8FC6D-0EC0-4248-B3D5-FB7AF54A2352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601E4F47-B1C5-554C-8168-3876ED1AD3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="6140" windowWidth="24600" windowHeight="17840" activeTab="1" xr2:uid="{352BA7F4-E16E-5A48-98CA-D2F763DC7C63}"/>
+    <workbookView xWindow="6140" yWindow="6140" windowWidth="24600" windowHeight="17840" activeTab="3" xr2:uid="{352BA7F4-E16E-5A48-98CA-D2F763DC7C63}"/>
   </bookViews>
   <sheets>
     <sheet name="chb01" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95280E7-387D-B545-B04F-0779BCC577D4}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -633,11 +635,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308F844B-8497-DB46-9000-62C318A5F004}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -739,7 +743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FA7D72-253A-E543-BB7F-957ABA0E6B76}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -845,7 +851,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6A1FA7-7423-294F-ACC1-EAECD4170566}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>